<commit_message>
Added DD Testing using xlsx file
</commit_message>
<xml_diff>
--- a/ninjaalgoproject/src/test/resources/TestData/loginData.xlsx
+++ b/ninjaalgoproject/src/test/resources/TestData/loginData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -23,13 +23,22 @@
     <t>Status</t>
   </si>
   <si>
+    <t>NinjaAlgo1</t>
+  </si>
+  <si>
+    <t>@Algo3</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
     <t>NinjaAlgo</t>
   </si>
   <si>
     <t>@Algo123</t>
   </si>
   <si>
-    <t>Valid</t>
+    <t>home</t>
   </si>
 </sst>
 </file>
@@ -74,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,6 +111,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>